<commit_message>
improved UI started adding playlist functionality
</commit_message>
<xml_diff>
--- a/proj_documentation/Final Project Mngmt Plan.xlsx
+++ b/proj_documentation/Final Project Mngmt Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobjanzen/Desktop/Fall_23/Database Management/final_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobjanzen/Desktop/Fall_23/Database Management/Streaming-Service-Final-Project/proj_documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFD5CE7-974E-B443-A05D-4ED2756FEB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E837F26E-7A0D-3D4A-90A8-29FFB787CCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1180" windowWidth="28040" windowHeight="17440" xr2:uid="{71ECD331-5348-9F48-B80E-A3AA5D273687}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Jobs</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Jacob, Noah</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -119,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -210,11 +219,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,37 +270,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -272,6 +314,50 @@
           <color indexed="64"/>
         </left>
         <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -314,22 +400,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -338,20 +408,18 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+        <left style="medium">
           <color indexed="64"/>
         </left>
-        <right style="thin">
+        <right style="medium">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -368,12 +436,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63F11225-74C8-FB49-8419-AC4BCFEC579D}" name="Table1" displayName="Table1" ref="A2:C12" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A2:C12" xr:uid="{63F11225-74C8-FB49-8419-AC4BCFEC579D}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{76829DC2-FA8C-0744-9A96-E357A3C7BD8C}" name="Final Project Management Schedule" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{9DC47874-E583-4B4D-9A71-62AA1F7A42F5}" name="Column1" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{1C11D2DA-D29D-2E45-9B99-F64F3DB1A29B}" name="Column2" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63F11225-74C8-FB49-8419-AC4BCFEC579D}" name="Table1" displayName="Table1" ref="A2:D12" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A2:D12" xr:uid="{63F11225-74C8-FB49-8419-AC4BCFEC579D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{76829DC2-FA8C-0744-9A96-E357A3C7BD8C}" name="Final Project Management Schedule" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{9DC47874-E583-4B4D-9A71-62AA1F7A42F5}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{1C11D2DA-D29D-2E45-9B99-F64F3DB1A29B}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{66C4984B-5A2A-784D-9684-8A95EA45F036}" name="Completed" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -676,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7249BF71-8FA8-1749-96BD-15366DF589F7}">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C12"/>
+      <selection activeCell="A2" sqref="A2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,125 +758,148 @@
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="11">
         <v>45246</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="11">
         <v>45254</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="11">
         <v>45254</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="11">
         <v>45258</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="11">
         <v>45258</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="11">
         <v>45258</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="10">
-        <v>45258</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="11">
         <v>45262</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="13">
         <v>45273</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restored past version from working tree
</commit_message>
<xml_diff>
--- a/proj_documentation/Final Project Mngmt Plan.xlsx
+++ b/proj_documentation/Final Project Mngmt Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobjanzen/Desktop/Fall_23/Database Management/Streaming-Service-Final-Project/proj_documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobjanzen/Desktop/Fall_23/Database Management/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E837F26E-7A0D-3D4A-90A8-29FFB787CCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFD5CE7-974E-B443-A05D-4ED2756FEB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1180" windowWidth="28040" windowHeight="17440" xr2:uid="{71ECD331-5348-9F48-B80E-A3AA5D273687}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Jobs</t>
   </si>
@@ -96,15 +96,6 @@
   </si>
   <si>
     <t>Jacob, Noah</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -128,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -219,39 +210,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -270,42 +233,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="7">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -314,50 +272,6 @@
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -400,6 +314,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -408,18 +338,20 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
+        <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="medium">
+        <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -436,13 +368,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63F11225-74C8-FB49-8419-AC4BCFEC579D}" name="Table1" displayName="Table1" ref="A2:D12" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A2:D12" xr:uid="{63F11225-74C8-FB49-8419-AC4BCFEC579D}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{76829DC2-FA8C-0744-9A96-E357A3C7BD8C}" name="Final Project Management Schedule" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{9DC47874-E583-4B4D-9A71-62AA1F7A42F5}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{1C11D2DA-D29D-2E45-9B99-F64F3DB1A29B}" name="Column2" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{66C4984B-5A2A-784D-9684-8A95EA45F036}" name="Completed" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63F11225-74C8-FB49-8419-AC4BCFEC579D}" name="Table1" displayName="Table1" ref="A2:C12" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A2:C12" xr:uid="{63F11225-74C8-FB49-8419-AC4BCFEC579D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{76829DC2-FA8C-0744-9A96-E357A3C7BD8C}" name="Final Project Management Schedule" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{9DC47874-E583-4B4D-9A71-62AA1F7A42F5}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{1C11D2DA-D29D-2E45-9B99-F64F3DB1A29B}" name="Column2" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -745,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7249BF71-8FA8-1749-96BD-15366DF589F7}">
-  <dimension ref="A2:D12"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D12"/>
+      <selection activeCell="A2" sqref="A2:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,148 +689,125 @@
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>45246</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>45254</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>45254</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>45258</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>45258</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>45258</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10">
+        <v>45258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>45262</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>45273</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>